<commit_message>
created global exception and tested user login and register through postman
</commit_message>
<xml_diff>
--- a/EMS_DB Design.xlsx
+++ b/EMS_DB Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EmployeeManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3793213-FC17-4AE9-AFB6-468DE17D6682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CF42B7-EE90-4E3A-9721-3ADC7AE9FE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="11660" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="173">
   <si>
     <t>Leave Tracker:</t>
   </si>
@@ -295,9 +295,6 @@
     <t>User(Data)</t>
   </si>
   <si>
-    <t>PendingUser(Data)</t>
-  </si>
-  <si>
     <t>PerfStatus</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>RoleUID</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -533,6 +527,18 @@
   </si>
   <si>
     <t>DisplayName</t>
+  </si>
+  <si>
+    <t>PasswordHash</t>
+  </si>
+  <si>
+    <t>HashKey</t>
+  </si>
+  <si>
+    <t>ResetPasswordToken</t>
+  </si>
+  <si>
+    <t>ResetPasswordTokenKey</t>
   </si>
 </sst>
 </file>
@@ -894,13 +900,13 @@
   </sheetPr>
   <dimension ref="A2:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>41</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>47</v>
       </c>
@@ -1342,12 +1348,10 @@
       <c r="A27" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>91</v>
-      </c>
+      <c r="D27" s="16"/>
       <c r="E27" s="17"/>
       <c r="G27" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>62</v>
@@ -1357,11 +1361,9 @@
       <c r="A28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D28" s="10"/>
       <c r="G28" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>62</v>
@@ -1369,11 +1371,9 @@
     </row>
     <row r="29" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>94</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D29" s="10"/>
       <c r="G29" s="10" t="s">
         <v>53</v>
       </c>
@@ -1383,295 +1383,253 @@
     </row>
     <row r="30" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>95</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>96</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>98</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="G33" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K33" s="15"/>
     </row>
     <row r="34" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>102</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D34" s="10"/>
       <c r="G34" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="G35" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I35" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D36" s="10"/>
       <c r="G36" s="10" t="s">
         <v>50</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>109</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D37" s="10"/>
       <c r="G37" s="10" t="s">
         <v>52</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>112</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="D38" s="10"/>
       <c r="G38" s="10" t="s">
         <v>54</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>115</v>
-      </c>
+      <c r="D39" s="10"/>
       <c r="G39" s="10" t="s">
         <v>57</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>118</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D40" s="10"/>
       <c r="G40" s="10" t="s">
         <v>60</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>120</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D41" s="10"/>
       <c r="G41" s="10" t="s">
         <v>64</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>122</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D42" s="10"/>
       <c r="G42" s="10" t="s">
         <v>66</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D43" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="G43" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G43" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>126</v>
-      </c>
       <c r="J43" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>127</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>79</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>84</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>128</v>
-      </c>
+      <c r="D47" s="10"/>
       <c r="F47" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="10" t="s">
-        <v>130</v>
-      </c>
+      <c r="D48" s="10"/>
       <c r="F48" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>131</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D49" s="10"/>
       <c r="F49" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>132</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D50" s="10"/>
       <c r="F50" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>79</v>
@@ -1679,7 +1637,7 @@
     </row>
     <row r="55" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>86</v>
@@ -1692,7 +1650,7 @@
     </row>
     <row r="57" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
@@ -1707,7 +1665,27 @@
     </row>
     <row r="60" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -1715,351 +1693,351 @@
         <v>13</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Payslip API and Database task completed
</commit_message>
<xml_diff>
--- a/EMS_DB Design.xlsx
+++ b/EMS_DB Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EmployeeManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CF42B7-EE90-4E3A-9721-3ADC7AE9FE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24ECC63-3F2E-4571-8501-3AC709A165CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="179">
   <si>
     <t>Leave Tracker:</t>
   </si>
@@ -316,9 +316,6 @@
     <t>PhNumber</t>
   </si>
   <si>
-    <t>Salary Details(data)</t>
-  </si>
-  <si>
     <t>Allowances:</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Allowance Name</t>
-  </si>
-  <si>
     <t>House Rent Allowance</t>
   </si>
   <si>
@@ -539,13 +533,37 @@
   </si>
   <si>
     <t>ResetPasswordTokenKey</t>
+  </si>
+  <si>
+    <t>Designation(config)</t>
+  </si>
+  <si>
+    <t>There is many to many relationship between Designation and Allowance.</t>
+  </si>
+  <si>
+    <t>Salary Structure(Data)</t>
+  </si>
+  <si>
+    <t>DesignationId</t>
+  </si>
+  <si>
+    <t>AllowanceId</t>
+  </si>
+  <si>
+    <t>Id,name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>AllowanceType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -597,6 +615,28 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -655,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -680,6 +720,9 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,8 +943,8 @@
   </sheetPr>
   <dimension ref="A2:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="E32" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1438,7 @@
     </row>
     <row r="32" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D32" s="10"/>
     </row>
@@ -1405,11 +1448,11 @@
       </c>
       <c r="D33" s="10"/>
       <c r="G33" s="19" t="s">
-        <v>98</v>
+        <v>171</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K33" s="15"/>
     </row>
@@ -1418,66 +1461,66 @@
         <v>97</v>
       </c>
       <c r="D34" s="10"/>
-      <c r="G34" s="10" t="s">
-        <v>13</v>
+      <c r="G34" s="24" t="s">
+        <v>176</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="10"/>
       <c r="G35" s="10" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="10"/>
       <c r="G36" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D37" s="10"/>
       <c r="G37" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D38" s="10"/>
       <c r="G38" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
@@ -1486,86 +1529,86 @@
       </c>
       <c r="D39" s="10"/>
       <c r="G39" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D40" s="10"/>
       <c r="G40" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D41" s="10"/>
       <c r="G41" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D43" s="10"/>
-      <c r="G43" s="10" t="s">
-        <v>123</v>
-      </c>
       <c r="I43" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D46" s="10"/>
+      <c r="G46" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
@@ -1573,10 +1616,10 @@
       </c>
       <c r="D47" s="10"/>
       <c r="F47" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="13" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>84</v>
       </c>
@@ -1584,108 +1627,126 @@
       <c r="F48" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G48" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D49" s="10"/>
       <c r="F49" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G49" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D50" s="10"/>
       <c r="F50" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F51" s="10" t="s">
+      <c r="G52" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" s="10" t="s">
+      <c r="F53" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="G53" s="23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -1693,21 +1754,21 @@
         <v>13</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -1715,10 +1776,10 @@
         <v>94</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -1726,65 +1787,65 @@
         <v>95</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -1792,255 +1853,256 @@
         <v>96</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>